<commit_message>
final config and all trials ran
</commit_message>
<xml_diff>
--- a/model_config_performance.xlsx
+++ b/model_config_performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Grad_School\Deep_Learning\cs5567_deep_learning_proj1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA7D2FF-D7C5-4A04-B432-15F9DAA952E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084FF810-CB73-4429-9AAE-3025E6E0D35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="375" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,7 +395,7 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+      <selection activeCell="G35" sqref="G31:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>